<commit_message>
multiple small fixes from feedback
</commit_message>
<xml_diff>
--- a/Data Sheets/Generic Kelp Clearing Data Sheet v1.4.xlsx
+++ b/Data Sheets/Generic Kelp Clearing Data Sheet v1.4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Site Info" sheetId="26" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="92512" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="97">
   <si>
     <t>Other Echinoids</t>
   </si>
@@ -214,14 +214,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>SL</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>HJ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Anemones</t>
   </si>
   <si>
@@ -314,18 +306,54 @@
   <si>
     <t xml:space="preserve">Sand (&gt;1cm)    </t>
   </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Ulva</t>
+  </si>
+  <si>
+    <t>Sargassum linearifolium</t>
+  </si>
+  <si>
+    <t>Sargassum vestitum</t>
+  </si>
+  <si>
+    <t>Lobophora variegata</t>
+  </si>
+  <si>
+    <t>Delisea pulchra</t>
+  </si>
+  <si>
+    <t>Peyssonnelia novae-hollandiae</t>
+  </si>
+  <si>
+    <t>Amphiroa anceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corallina officinalis </t>
+  </si>
+  <si>
+    <t>Jania</t>
+  </si>
+  <si>
+    <t>Filamenteous turf</t>
+  </si>
+  <si>
+    <t>Crustose coralline algae (CCA)</t>
+  </si>
+  <si>
+    <t>Codium</t>
+  </si>
+  <si>
+    <t>Sabellidae (Fan worm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="42">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -864,325 +892,325 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1191,42 +1219,42 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1234,81 +1262,81 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1657,6 +1685,18 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1691,18 +1731,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1715,12 +1749,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1728,7 +1756,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -6418,17 +6446,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
@@ -6437,20 +6465,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="33" customFormat="1" ht="16" customHeight="1">
-      <c r="B1" s="154" t="s">
+      <c r="B1" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154" t="s">
+      <c r="C1" s="166"/>
+      <c r="D1" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="162" t="s">
-        <v>59</v>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="174" t="s">
+        <v>57</v>
       </c>
-      <c r="I1" s="155"/>
+      <c r="I1" s="167"/>
       <c r="J1" s="144"/>
       <c r="K1" s="144"/>
       <c r="L1" s="144"/>
@@ -6459,14 +6487,14 @@
       <c r="O1" s="144"/>
     </row>
     <row r="2" spans="1:15" s="33" customFormat="1" ht="16" customHeight="1">
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
       <c r="J2" s="144"/>
       <c r="K2" s="144"/>
       <c r="L2" s="144"/>
@@ -6507,22 +6535,22 @@
     <row r="5" spans="1:15" s="29" customFormat="1" ht="34" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="140"/>
       <c r="B5" s="141"/>
-      <c r="C5" s="156" t="s">
+      <c r="C5" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="157"/>
-      <c r="E5" s="158" t="s">
+      <c r="D5" s="169"/>
+      <c r="E5" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="159"/>
-      <c r="G5" s="160" t="s">
+      <c r="F5" s="171"/>
+      <c r="G5" s="172" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="161"/>
-      <c r="I5" s="158" t="s">
+      <c r="H5" s="173"/>
+      <c r="I5" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="159"/>
+      <c r="J5" s="171"/>
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
@@ -6533,14 +6561,14 @@
       <c r="B6" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="153"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="165"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -6551,14 +6579,14 @@
       <c r="B7" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="166"/>
+      <c r="C7" s="159"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="160"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
@@ -6569,14 +6597,14 @@
       <c r="B8" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="163"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="163"/>
-      <c r="H8" s="164"/>
-      <c r="I8" s="163"/>
-      <c r="J8" s="164"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="158"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
@@ -6587,14 +6615,14 @@
       <c r="B9" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="163"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="163"/>
-      <c r="H9" s="164"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="164"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="158"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="158"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
@@ -6605,14 +6633,14 @@
       <c r="B10" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="163"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="164"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="164"/>
-      <c r="I10" s="163"/>
-      <c r="J10" s="164"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="158"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="158"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
@@ -6623,14 +6651,14 @@
       <c r="B11" s="148" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="167"/>
-      <c r="D11" s="168"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="167"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="167"/>
-      <c r="J11" s="168"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="162"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="162"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="162"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
@@ -6641,14 +6669,14 @@
       <c r="B12" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="165"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="165"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="165"/>
-      <c r="J12" s="166"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="159"/>
+      <c r="F12" s="160"/>
+      <c r="G12" s="159"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="159"/>
+      <c r="J12" s="160"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
@@ -6659,14 +6687,14 @@
       <c r="B13" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="164"/>
-      <c r="E13" s="163"/>
-      <c r="F13" s="164"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="164"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="164"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="158"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="158"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="158"/>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -6677,14 +6705,14 @@
       <c r="B14" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="163"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="163"/>
-      <c r="F14" s="164"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="164"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="164"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="158"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="158"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -6695,14 +6723,14 @@
       <c r="B15" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="163"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="163"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="164"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="164"/>
+      <c r="C15" s="157"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="157"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="157"/>
+      <c r="H15" s="158"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="158"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -6713,14 +6741,14 @@
       <c r="B16" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="167"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="167"/>
-      <c r="F16" s="168"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="168"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="168"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="162"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="162"/>
+      <c r="G16" s="161"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="161"/>
+      <c r="J16" s="162"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -6731,14 +6759,14 @@
       <c r="B17" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="166"/>
-      <c r="E17" s="165"/>
-      <c r="F17" s="166"/>
-      <c r="G17" s="165"/>
-      <c r="H17" s="166"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="166"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="160"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="159"/>
+      <c r="J17" s="160"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -6749,14 +6777,14 @@
       <c r="B18" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="163"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="163"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="164"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="164"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="158"/>
+      <c r="G18" s="157"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="157"/>
+      <c r="J18" s="158"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -6767,14 +6795,14 @@
       <c r="B19" s="148" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="163"/>
-      <c r="D19" s="164"/>
-      <c r="E19" s="163"/>
-      <c r="F19" s="164"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="164"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="164"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="157"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="157"/>
+      <c r="J19" s="158"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -6785,14 +6813,14 @@
       <c r="B20" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="169"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="170"/>
+      <c r="C20" s="151"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="152"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -6801,14 +6829,14 @@
     <row r="21" spans="1:14" s="29" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="A21" s="140"/>
       <c r="B21" s="142"/>
-      <c r="C21" s="171"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="171"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="171"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="171"/>
-      <c r="J21" s="172"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="153"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="153"/>
+      <c r="H21" s="154"/>
+      <c r="I21" s="153"/>
+      <c r="J21" s="154"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -6817,14 +6845,14 @@
     <row r="22" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A22" s="140"/>
       <c r="B22" s="139"/>
-      <c r="C22" s="171"/>
-      <c r="D22" s="172"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="172"/>
+      <c r="C22" s="153"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="153"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="153"/>
+      <c r="H22" s="154"/>
+      <c r="I22" s="153"/>
+      <c r="J22" s="154"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -6833,14 +6861,14 @@
     <row r="23" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A23" s="140"/>
       <c r="B23" s="138"/>
-      <c r="C23" s="171"/>
-      <c r="D23" s="172"/>
-      <c r="E23" s="171"/>
-      <c r="F23" s="172"/>
-      <c r="G23" s="171"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="171"/>
-      <c r="J23" s="172"/>
+      <c r="C23" s="153"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="154"/>
+      <c r="I23" s="153"/>
+      <c r="J23" s="154"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -6849,14 +6877,14 @@
     <row r="24" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A24" s="140"/>
       <c r="B24" s="138"/>
-      <c r="C24" s="171"/>
-      <c r="D24" s="172"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="172"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="154"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="154"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="154"/>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
@@ -6865,14 +6893,14 @@
     <row r="25" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A25" s="140"/>
       <c r="B25" s="138"/>
-      <c r="C25" s="171"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="171"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="171"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="171"/>
-      <c r="J25" s="172"/>
+      <c r="C25" s="153"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="153"/>
+      <c r="H25" s="154"/>
+      <c r="I25" s="153"/>
+      <c r="J25" s="154"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
@@ -6881,14 +6909,14 @@
     <row r="26" spans="1:14" s="29" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="A26" s="140"/>
       <c r="B26" s="142"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="172"/>
-      <c r="E26" s="171"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="171"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="172"/>
+      <c r="C26" s="153"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="154"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="153"/>
+      <c r="J26" s="154"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -6897,14 +6925,14 @@
     <row r="27" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A27" s="140"/>
       <c r="B27" s="139"/>
-      <c r="C27" s="171"/>
-      <c r="D27" s="172"/>
-      <c r="E27" s="171"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="171"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="171"/>
-      <c r="J27" s="172"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="154"/>
+      <c r="I27" s="153"/>
+      <c r="J27" s="154"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -6913,14 +6941,14 @@
     <row r="28" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A28" s="140"/>
       <c r="B28" s="138"/>
-      <c r="C28" s="171"/>
-      <c r="D28" s="172"/>
-      <c r="E28" s="171"/>
-      <c r="F28" s="172"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="172"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="154"/>
+      <c r="I28" s="153"/>
+      <c r="J28" s="154"/>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -6929,14 +6957,14 @@
     <row r="29" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A29" s="140"/>
       <c r="B29" s="138"/>
-      <c r="C29" s="171"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="171"/>
-      <c r="F29" s="172"/>
-      <c r="G29" s="171"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="171"/>
-      <c r="J29" s="172"/>
+      <c r="C29" s="153"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="153"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="154"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="154"/>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -6945,14 +6973,14 @@
     <row r="30" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A30" s="140"/>
       <c r="B30" s="138"/>
-      <c r="C30" s="171"/>
-      <c r="D30" s="172"/>
-      <c r="E30" s="171"/>
-      <c r="F30" s="172"/>
-      <c r="G30" s="171"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="171"/>
-      <c r="J30" s="172"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="154"/>
+      <c r="E30" s="153"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="153"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="154"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -6961,14 +6989,14 @@
     <row r="31" spans="1:14" s="29" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="A31" s="140"/>
       <c r="B31" s="142"/>
-      <c r="C31" s="171"/>
-      <c r="D31" s="172"/>
-      <c r="E31" s="171"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="171"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="171"/>
-      <c r="J31" s="172"/>
+      <c r="C31" s="153"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="154"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
@@ -6977,14 +7005,14 @@
     <row r="32" spans="1:14" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A32" s="140"/>
       <c r="B32" s="139"/>
-      <c r="C32" s="171"/>
-      <c r="D32" s="172"/>
-      <c r="E32" s="171"/>
-      <c r="F32" s="172"/>
-      <c r="G32" s="171"/>
-      <c r="H32" s="172"/>
-      <c r="I32" s="171"/>
-      <c r="J32" s="172"/>
+      <c r="C32" s="153"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="153"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="154"/>
+      <c r="I32" s="153"/>
+      <c r="J32" s="154"/>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
@@ -6993,14 +7021,14 @@
     <row r="33" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A33" s="140"/>
       <c r="B33" s="138"/>
-      <c r="C33" s="171"/>
-      <c r="D33" s="172"/>
-      <c r="E33" s="171"/>
-      <c r="F33" s="172"/>
-      <c r="G33" s="171"/>
-      <c r="H33" s="172"/>
-      <c r="I33" s="171"/>
-      <c r="J33" s="172"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="154"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="154"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="154"/>
+      <c r="I33" s="153"/>
+      <c r="J33" s="154"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -7009,14 +7037,14 @@
     <row r="34" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A34" s="140"/>
       <c r="B34" s="138"/>
-      <c r="C34" s="171"/>
-      <c r="D34" s="172"/>
-      <c r="E34" s="171"/>
-      <c r="F34" s="172"/>
-      <c r="G34" s="171"/>
-      <c r="H34" s="172"/>
-      <c r="I34" s="171"/>
-      <c r="J34" s="172"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="154"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="154"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="154"/>
+      <c r="I34" s="153"/>
+      <c r="J34" s="154"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -7025,14 +7053,14 @@
     <row r="35" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A35" s="140"/>
       <c r="B35" s="138"/>
-      <c r="C35" s="171"/>
-      <c r="D35" s="172"/>
-      <c r="E35" s="171"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="171"/>
-      <c r="H35" s="172"/>
-      <c r="I35" s="171"/>
-      <c r="J35" s="172"/>
+      <c r="C35" s="153"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="153"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="154"/>
+      <c r="I35" s="153"/>
+      <c r="J35" s="154"/>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -7041,14 +7069,14 @@
     <row r="36" spans="1:18" s="29" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="A36" s="140"/>
       <c r="B36" s="142"/>
-      <c r="C36" s="171"/>
-      <c r="D36" s="172"/>
-      <c r="E36" s="171"/>
-      <c r="F36" s="172"/>
-      <c r="G36" s="171"/>
-      <c r="H36" s="172"/>
-      <c r="I36" s="171"/>
-      <c r="J36" s="172"/>
+      <c r="C36" s="153"/>
+      <c r="D36" s="154"/>
+      <c r="E36" s="153"/>
+      <c r="F36" s="154"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="154"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="154"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -7057,14 +7085,14 @@
     <row r="37" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A37" s="140"/>
       <c r="B37" s="139"/>
-      <c r="C37" s="171"/>
-      <c r="D37" s="172"/>
-      <c r="E37" s="171"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="171"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="171"/>
-      <c r="J37" s="172"/>
+      <c r="C37" s="153"/>
+      <c r="D37" s="154"/>
+      <c r="E37" s="153"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="154"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="154"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -7073,14 +7101,14 @@
     <row r="38" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A38" s="140"/>
       <c r="B38" s="138"/>
-      <c r="C38" s="171"/>
-      <c r="D38" s="172"/>
-      <c r="E38" s="171"/>
-      <c r="F38" s="172"/>
-      <c r="G38" s="171"/>
-      <c r="H38" s="172"/>
-      <c r="I38" s="171"/>
-      <c r="J38" s="172"/>
+      <c r="C38" s="153"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="153"/>
+      <c r="F38" s="154"/>
+      <c r="G38" s="153"/>
+      <c r="H38" s="154"/>
+      <c r="I38" s="153"/>
+      <c r="J38" s="154"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -7089,14 +7117,14 @@
     <row r="39" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A39" s="140"/>
       <c r="B39" s="138"/>
-      <c r="C39" s="171"/>
-      <c r="D39" s="172"/>
-      <c r="E39" s="171"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="171"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="171"/>
-      <c r="J39" s="172"/>
+      <c r="C39" s="153"/>
+      <c r="D39" s="154"/>
+      <c r="E39" s="153"/>
+      <c r="F39" s="154"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="154"/>
+      <c r="I39" s="153"/>
+      <c r="J39" s="154"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -7105,14 +7133,14 @@
     <row r="40" spans="1:18" s="29" customFormat="1" ht="16" thickTop="1">
       <c r="A40" s="140"/>
       <c r="B40" s="138"/>
-      <c r="C40" s="171"/>
-      <c r="D40" s="172"/>
-      <c r="E40" s="171"/>
-      <c r="F40" s="172"/>
-      <c r="G40" s="171"/>
-      <c r="H40" s="172"/>
-      <c r="I40" s="171"/>
-      <c r="J40" s="172"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="154"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="154"/>
+      <c r="G40" s="153"/>
+      <c r="H40" s="154"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="154"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -7121,14 +7149,14 @@
     <row r="41" spans="1:18" s="29" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="A41" s="140"/>
       <c r="B41" s="142"/>
-      <c r="C41" s="173"/>
-      <c r="D41" s="174"/>
-      <c r="E41" s="173"/>
-      <c r="F41" s="174"/>
-      <c r="G41" s="173"/>
-      <c r="H41" s="174"/>
-      <c r="I41" s="173"/>
-      <c r="J41" s="174"/>
+      <c r="C41" s="155"/>
+      <c r="D41" s="156"/>
+      <c r="E41" s="155"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="155"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="155"/>
+      <c r="J41" s="156"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -7622,62 +7650,6 @@
     <row r="86" ht="9.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="C20:D41"/>
-    <mergeCell ref="E20:F41"/>
-    <mergeCell ref="G20:H41"/>
-    <mergeCell ref="I20:J41"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
@@ -7689,6 +7661,62 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="H1:I2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C20:D41"/>
+    <mergeCell ref="E20:F41"/>
+    <mergeCell ref="G20:H41"/>
+    <mergeCell ref="I20:J41"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -7699,7 +7727,7 @@
     <oddFooter>&amp;LData entry by: ____________________x000D_Date entered: _____________________x000D_&amp;CChecked by: ______________________x000D_Date checked: ____________________x000D_&amp;R&amp;"Arial,Italic"&amp;6&amp;K3366FFupdated &amp;D</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -7707,7 +7735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7717,7 +7745,7 @@
       <selection activeCell="E59" sqref="E59:I66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
@@ -7726,47 +7754,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="33" customFormat="1" ht="12" customHeight="1">
-      <c r="B1" s="154" t="s">
+      <c r="B1" s="166" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="154"/>
-      <c r="D1" s="177" t="s">
+      <c r="C1" s="166"/>
+      <c r="D1" s="179" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="178" t="s">
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="154" t="s">
-        <v>61</v>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="166" t="s">
+        <v>59</v>
       </c>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="175" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="176"/>
-      <c r="O1" s="47"/>
-    </row>
-    <row r="2" spans="1:15" s="33" customFormat="1" ht="12" customHeight="1">
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="175" t="s">
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="177" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="176"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="47"/>
+    </row>
+    <row r="2" spans="1:15" s="33" customFormat="1" ht="12" customHeight="1">
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="177" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="178"/>
       <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" s="67" customFormat="1" ht="16" customHeight="1">
@@ -7775,7 +7803,7 @@
       </c>
       <c r="E3" s="86"/>
       <c r="G3" s="76" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="75"/>
       <c r="I3" s="75"/>
@@ -7802,10 +7830,10 @@
       <c r="N4" s="71"/>
     </row>
     <row r="5" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="179" t="s">
+      <c r="A5" s="175" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="180"/>
+      <c r="B5" s="176"/>
       <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
@@ -8442,7 +8470,7 @@
       <c r="D43" s="63"/>
       <c r="E43" s="64"/>
       <c r="F43" s="66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
@@ -8920,7 +8948,7 @@
     <oddFooter>&amp;LData entry by: ____________________x000D_Date entered: ____________________&amp;CChecked by: ______________________x000D_Date checked: ___________________&amp;R&amp;"Arial,Italic"&amp;6Updated &amp;D</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8928,63 +8956,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:M2"/>
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="13" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13">
-      <c r="A1" s="154" t="s">
-        <v>46</v>
+      <c r="A1" s="166" t="s">
+        <v>83</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="177" t="s">
+      <c r="B1" s="166"/>
+      <c r="C1" s="179" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="178" t="s">
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="154" t="s">
-        <v>61</v>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="166" t="s">
+        <v>59</v>
       </c>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="175" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="176"/>
-    </row>
-    <row r="2" spans="1:13" ht="13">
-      <c r="A2" s="154"/>
-      <c r="B2" s="154"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="175" t="s">
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="177" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="176"/>
+      <c r="M1" s="178"/>
+    </row>
+    <row r="2" spans="1:13" ht="13">
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="177" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="178"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="76" t="s">
@@ -8995,7 +9023,7 @@
       <c r="D3" s="86"/>
       <c r="E3" s="67"/>
       <c r="F3" s="76" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G3" s="75"/>
       <c r="H3" s="75"/>
@@ -9064,9 +9092,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="14" thickTop="1" thickBot="1">
-      <c r="A6" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="A6" s="9"/>
       <c r="B6" s="7"/>
       <c r="C6" s="82"/>
       <c r="D6" s="97"/>
@@ -9081,9 +9107,7 @@
       <c r="M6" s="82"/>
     </row>
     <row r="7" spans="1:13" ht="16" thickTop="1">
-      <c r="A7" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A7" s="9"/>
       <c r="B7" s="6"/>
       <c r="C7" s="80"/>
       <c r="D7" s="98"/>
@@ -9609,7 +9633,7 @@
     </row>
     <row r="42" spans="1:13" ht="16" thickTop="1">
       <c r="A42" s="136" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="87"/>
@@ -9626,7 +9650,7 @@
     </row>
     <row r="43" spans="1:13" ht="16" thickTop="1">
       <c r="A43" s="136" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="87"/>
@@ -9643,7 +9667,7 @@
     </row>
     <row r="44" spans="1:13" ht="16" thickTop="1">
       <c r="A44" s="136" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="87"/>
@@ -9660,7 +9684,7 @@
     </row>
     <row r="45" spans="1:13" ht="16" thickTop="1">
       <c r="A45" s="136" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="87"/>
@@ -9677,7 +9701,7 @@
     </row>
     <row r="46" spans="1:13" ht="17" thickTop="1" thickBot="1">
       <c r="A46" s="137" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="79"/>
@@ -9731,13 +9755,13 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="88" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="89" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;LKEEN Region_x000D_KEEN Lab PI_x000D_Area using this sheet&amp;C&amp;"Arial Narrow,Bold"&amp;12KEEN Kelp Removal Experiment_x000D_UPC Data Sheet&amp;RScanned by: _____________________x000D_Date scanned: __________________</oddHeader>
     <oddFooter>&amp;LData entry by: ____________________x000D_Date entered: ____________________&amp;CChecked by: ______________________x000D_Date checked: ___________________&amp;RUpdated &amp;D</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -9745,17 +9769,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CX107"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:Q64"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="AY16" sqref="AY16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="1.5" defaultRowHeight="7.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="1.5" defaultRowHeight="7.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="14" customWidth="1"/>
     <col min="2" max="6" width="1.5" style="27"/>
@@ -9858,7 +9882,7 @@
       <c r="AR2" s="107"/>
       <c r="AS2" s="107"/>
       <c r="AT2" s="112" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AU2" s="111"/>
       <c r="AV2" s="107"/>
@@ -9917,10 +9941,10 @@
       <c r="AP3" s="105"/>
       <c r="AQ3" s="107"/>
       <c r="AR3" s="113" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AS3" s="107" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AT3" s="107"/>
       <c r="AU3" s="111"/>
@@ -9929,10 +9953,10 @@
       <c r="AX3" s="107"/>
       <c r="AY3" s="107"/>
       <c r="BC3" s="113" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="BD3" s="107" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BE3" s="107"/>
       <c r="BF3" s="107"/>
@@ -9987,10 +10011,10 @@
       <c r="AP4" s="105"/>
       <c r="AQ4" s="107"/>
       <c r="AR4" s="113" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AS4" s="107" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AT4" s="107"/>
       <c r="AU4" s="111"/>
@@ -9999,10 +10023,10 @@
       <c r="AX4" s="107"/>
       <c r="AY4" s="107"/>
       <c r="BC4" s="103" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="BD4" s="107" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="BE4" s="107"/>
       <c r="BF4" s="118"/>
@@ -10014,7 +10038,9 @@
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5"/>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
@@ -10055,10 +10081,10 @@
       <c r="AP5" s="105"/>
       <c r="AQ5" s="107"/>
       <c r="AR5" s="113" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AS5" s="107" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AT5" s="107"/>
       <c r="AU5" s="111"/>
@@ -10067,10 +10093,10 @@
       <c r="AX5" s="107"/>
       <c r="AY5" s="107"/>
       <c r="BC5" s="103" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BD5" s="107" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BE5" s="107"/>
       <c r="BF5" s="107"/>
@@ -10082,7 +10108,9 @@
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
-      <c r="D6"/>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
@@ -10125,10 +10153,10 @@
       <c r="AP6" s="105"/>
       <c r="AQ6" s="107"/>
       <c r="AR6" s="109" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AS6" s="104" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AT6" s="107"/>
       <c r="AU6" s="111"/>
@@ -10137,10 +10165,10 @@
       <c r="AX6" s="107"/>
       <c r="AY6" s="107"/>
       <c r="BC6" s="113" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="BD6" s="107" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="BE6" s="107"/>
       <c r="BF6" s="107"/>
@@ -10745,7 +10773,9 @@
       <c r="AV16"/>
       <c r="AW16"/>
       <c r="AX16"/>
-      <c r="AY16"/>
+      <c r="AY16" t="s">
+        <v>96</v>
+      </c>
       <c r="AZ16"/>
       <c r="BA16"/>
       <c r="BB16"/>
@@ -10938,7 +10968,7 @@
       <c r="AX19" s="107"/>
       <c r="AY19" s="19"/>
       <c r="AZ19" s="102" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="BA19" s="103"/>
       <c r="BB19" s="107"/>
@@ -11442,7 +11472,9 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27"/>
+      <c r="D27" t="s">
+        <v>88</v>
+      </c>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
@@ -11510,7 +11542,9 @@
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28"/>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
@@ -11576,7 +11610,9 @@
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
-      <c r="D29"/>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
@@ -11641,7 +11677,9 @@
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
-      <c r="D30"/>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
@@ -11704,7 +11742,9 @@
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31"/>
+      <c r="D31" t="s">
+        <v>92</v>
+      </c>
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
@@ -11767,7 +11807,9 @@
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
-      <c r="D32"/>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
@@ -11830,7 +11872,9 @@
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
-      <c r="D33"/>
+      <c r="D33" t="s">
+        <v>94</v>
+      </c>
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
@@ -12084,7 +12128,9 @@
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
-      <c r="D37"/>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
@@ -12147,7 +12193,9 @@
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
-      <c r="D38"/>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
@@ -12210,7 +12258,9 @@
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
-      <c r="D39"/>
+      <c r="D39" t="s">
+        <v>87</v>
+      </c>
       <c r="E39"/>
       <c r="F39"/>
       <c r="G39"/>
@@ -14922,14 +14972,14 @@
   </sheetData>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.56999999999999995" right="0.5" top="0.52" bottom="0.52" header="0.15" footer="0.15"/>
-  <pageSetup scale="81" orientation="portrait"/>
+  <pageSetup scale="80" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;8KEEN REGION_x000D_KEEN Lab PI_x000D_Area Using This List&amp;C&amp;"Arial,Bold"&amp;12 Sample UNIFORM POINT CONTACT_x000D_SPECIES LIST_x000D_</oddHeader>
     <oddFooter>&amp;R&amp;8Updated &amp;D</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -14937,19 +14987,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>